<commit_message>
Align WHO Measles and HPV with current WHO guidance
- Measles: split into two series for different country schedules —
  9-month first dose (dose 2 at 15mo) and 12-month first dose (dose 2
  at 4y school entry). Fix dose 2 absMinAge based on interval, remove
  latestRecAge caps, preserve lab immunity criterion
- HPV: extend single-dose maxAge from 15y to 20y per WHO 2022 SAGE,
  change two-dose series from 15y to 21y threshold, add three-dose
  immunocompromised risk series (obs 1022)

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/cicada_generator/lib/WHO/antigen/HPV.xlsx
+++ b/cicada_generator/lib/WHO/antigen/HPV.xlsx
@@ -6,6 +6,7 @@
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="1-dose series" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="2-dose series" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="3-dose series (immunocompromised)" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -13,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="48">
   <si>
     <t xml:space="preserve">Series Name</t>
   </si>
@@ -66,7 +67,7 @@
     <t xml:space="preserve">9 years</t>
   </si>
   <si>
-    <t xml:space="preserve">15 years</t>
+    <t xml:space="preserve">20 years</t>
   </si>
   <si>
     <t xml:space="preserve">Series Dose</t>
@@ -102,18 +103,18 @@
     <t xml:space="preserve">Recurring Dose</t>
   </si>
   <si>
-    <t xml:space="preserve">WHO HPV 2-dose series (&gt;=15y)</t>
+    <t xml:space="preserve">WHO HPV 2-dose series (&gt;=21y)</t>
   </si>
   <si>
     <t xml:space="preserve">2</t>
   </si>
   <si>
+    <t xml:space="preserve">21 years</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dose 2</t>
   </si>
   <si>
-    <t xml:space="preserve">15 years + 5 months</t>
-  </si>
-  <si>
     <t xml:space="preserve">Preferable Interval</t>
   </si>
   <si>
@@ -121,6 +122,42 @@
   </si>
   <si>
     <t xml:space="preserve">6 months</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHO HPV 3-dose series (immunocompromised)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Risk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Immunocompromised</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Immunocompromised individual (1022)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient is immunocompromised — requires 3-dose HPV series</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 weeks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 months</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dose 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 weeks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 months</t>
   </si>
 </sst>
 </file>
@@ -485,12 +522,6 @@
       <c r="F9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
@@ -648,7 +679,7 @@
         <v>30</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>8</v>
@@ -670,21 +701,15 @@
         <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -766,33 +791,324 @@
         <v>18</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
         <v>20</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="17">
@@ -812,24 +1128,15 @@
         <v>8</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L17" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -903,6 +1210,116 @@
         <v>28</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>